<commit_message>
Redid scaling in multilinearreg file
</commit_message>
<xml_diff>
--- a/Final EU Data.xlsx
+++ b/Final EU Data.xlsx
@@ -518,16 +518,16 @@
         <v>3163147.9</v>
       </c>
       <c r="I2" t="n">
-        <v>197274.5995016437</v>
+        <v>150991.8164123378</v>
       </c>
       <c r="J2" t="n">
-        <v>290415.1696993739</v>
+        <v>322916.2541075106</v>
       </c>
       <c r="K2" t="n">
-        <v>222913.5876905106</v>
+        <v>175139.8326550492</v>
       </c>
       <c r="L2" t="n">
-        <v>312519.848929872</v>
+        <v>344977.530106144</v>
       </c>
     </row>
     <row r="3">
@@ -558,16 +558,16 @@
         <v>9946647.699999999</v>
       </c>
       <c r="I3" t="n">
-        <v>694155.4821261413</v>
+        <v>619340.4399868009</v>
       </c>
       <c r="J3" t="n">
-        <v>850624.7941116695</v>
+        <v>904148.1533773908</v>
       </c>
       <c r="K3" t="n">
-        <v>731920.1442377389</v>
+        <v>654908.9915752509</v>
       </c>
       <c r="L3" t="n">
-        <v>883183.6352046069</v>
+        <v>936643.0641633343</v>
       </c>
     </row>
     <row r="4">
@@ -598,16 +598,16 @@
         <v>12787486.8</v>
       </c>
       <c r="I4" t="n">
-        <v>898978.1859046598</v>
+        <v>911249.6041315054</v>
       </c>
       <c r="J4" t="n">
-        <v>1031987.2140688</v>
+        <v>1049684.73976003</v>
       </c>
       <c r="K4" t="n">
-        <v>924818.5906718895</v>
+        <v>935587.324069621</v>
       </c>
       <c r="L4" t="n">
-        <v>1054265.544803157</v>
+        <v>1071919.326292341</v>
       </c>
     </row>
     <row r="5">
@@ -638,16 +638,16 @@
         <v>3593093.9</v>
       </c>
       <c r="I5" t="n">
-        <v>248364.6496526078</v>
+        <v>179929.469339055</v>
       </c>
       <c r="J5" t="n">
-        <v>320448.7963664928</v>
+        <v>357553.6942982785</v>
       </c>
       <c r="K5" t="n">
-        <v>276259.2170620622</v>
+        <v>206201.8971714219</v>
       </c>
       <c r="L5" t="n">
-        <v>344498.1254709557</v>
+        <v>381555.8017897776</v>
       </c>
     </row>
     <row r="6">
@@ -678,16 +678,16 @@
         <v>4496184</v>
       </c>
       <c r="I6" t="n">
-        <v>302952.3975664166</v>
+        <v>246934.8822290114</v>
       </c>
       <c r="J6" t="n">
-        <v>392708.4700635311</v>
+        <v>428211.9206647582</v>
       </c>
       <c r="K6" t="n">
-        <v>332532.7774073413</v>
+        <v>274795.0882403546</v>
       </c>
       <c r="L6" t="n">
-        <v>418211.2240366329</v>
+        <v>453664.599179522</v>
       </c>
     </row>
     <row r="7">
@@ -718,16 +718,16 @@
         <v>1334864.3</v>
       </c>
       <c r="I7" t="n">
-        <v>35433.91850059403</v>
+        <v>-28459.16983042323</v>
       </c>
       <c r="J7" t="n">
-        <v>256038.253035158</v>
+        <v>316261.1672119474</v>
       </c>
       <c r="K7" t="n">
-        <v>23577.93792973361</v>
+        <v>-39625.69517414671</v>
       </c>
       <c r="L7" t="n">
-        <v>245816.6075649328</v>
+        <v>306059.5922636129</v>
       </c>
     </row>
     <row r="8">
@@ -758,16 +758,16 @@
         <v>11795218.6</v>
       </c>
       <c r="I8" t="n">
-        <v>834485.9225663096</v>
+        <v>784943.8744965211</v>
       </c>
       <c r="J8" t="n">
-        <v>1006948.457310016</v>
+        <v>1053879.66278772</v>
       </c>
       <c r="K8" t="n">
-        <v>855040.9221328525</v>
+        <v>804303.5489011975</v>
       </c>
       <c r="L8" t="n">
-        <v>1024669.970680765</v>
+        <v>1071566.379410422</v>
       </c>
     </row>
     <row r="9">
@@ -798,16 +798,16 @@
         <v>6387489.9</v>
       </c>
       <c r="I9" t="n">
-        <v>509668.0383275302</v>
+        <v>462666.2129662216</v>
       </c>
       <c r="J9" t="n">
-        <v>776928.110872409</v>
+        <v>838746.6093900969</v>
       </c>
       <c r="K9" t="n">
-        <v>374245.6772919919</v>
+        <v>335119.0044015516</v>
       </c>
       <c r="L9" t="n">
-        <v>660173.5872821555</v>
+        <v>722221.336973579</v>
       </c>
     </row>
     <row r="10">
@@ -838,16 +838,16 @@
         <v>1459877.1</v>
       </c>
       <c r="I10" t="n">
-        <v>49228.48181717054</v>
+        <v>4161.713205915598</v>
       </c>
       <c r="J10" t="n">
-        <v>214657.0475872133</v>
+        <v>258774.6683200491</v>
       </c>
       <c r="K10" t="n">
-        <v>53291.66598356119</v>
+        <v>7988.612946434011</v>
       </c>
       <c r="L10" t="n">
-        <v>218160.1258674827</v>
+        <v>262270.8681961013</v>
       </c>
     </row>
     <row r="11">
@@ -878,16 +878,16 @@
         <v>6101438.2</v>
       </c>
       <c r="I11" t="n">
-        <v>359182.4321205182</v>
+        <v>333039.6142924197</v>
       </c>
       <c r="J11" t="n">
-        <v>573414.9081220827</v>
+        <v>618741.7211936882</v>
       </c>
       <c r="K11" t="n">
-        <v>383359.8358206981</v>
+        <v>355811.0408775005</v>
       </c>
       <c r="L11" t="n">
-        <v>594259.4808283801</v>
+        <v>639545.3649268548</v>
       </c>
     </row>
     <row r="12">
@@ -918,16 +918,16 @@
         <v>71912361.40000001</v>
       </c>
       <c r="I12" t="n">
-        <v>5437676.776423956</v>
+        <v>5339047.169138927</v>
       </c>
       <c r="J12" t="n">
-        <v>5550810.871076449</v>
+        <v>5605829.629295891</v>
       </c>
       <c r="K12" t="n">
-        <v>5579369.066092212</v>
+        <v>5472499.694143863</v>
       </c>
       <c r="L12" t="n">
-        <v>5672971.019888859</v>
+        <v>5727749.91281968</v>
       </c>
     </row>
     <row r="13">
@@ -958,16 +958,16 @@
         <v>92369061.40000001</v>
       </c>
       <c r="I13" t="n">
-        <v>6717938.457309463</v>
+        <v>6584437.838945085</v>
       </c>
       <c r="J13" t="n">
-        <v>6927584.841623625</v>
+        <v>7011485.666034247</v>
       </c>
       <c r="K13" t="n">
-        <v>7162385.298904049</v>
+        <v>7003038.973700793</v>
       </c>
       <c r="L13" t="n">
-        <v>7310765.129242084</v>
+        <v>7393913.567124221</v>
       </c>
     </row>
     <row r="14">
@@ -998,16 +998,16 @@
         <v>11425943.1</v>
       </c>
       <c r="I14" t="n">
-        <v>783049.8053638649</v>
+        <v>756767.4396967822</v>
       </c>
       <c r="J14" t="n">
-        <v>919505.5865565595</v>
+        <v>951905.5567331358</v>
       </c>
       <c r="K14" t="n">
-        <v>836802.2506499827</v>
+        <v>807394.0444712352</v>
       </c>
       <c r="L14" t="n">
-        <v>965848.3108540992</v>
+        <v>998157.2856361279</v>
       </c>
     </row>
     <row r="15">
@@ -1038,16 +1038,16 @@
         <v>10607413.3</v>
       </c>
       <c r="I15" t="n">
-        <v>719375.6416698351</v>
+        <v>680879.6059397161</v>
       </c>
       <c r="J15" t="n">
-        <v>850231.1532559381</v>
+        <v>886172.1217645985</v>
       </c>
       <c r="K15" t="n">
-        <v>782139.4512948948</v>
+        <v>739993.5414474566</v>
       </c>
       <c r="L15" t="n">
-        <v>904343.0343031173</v>
+        <v>940177.7524339625</v>
       </c>
     </row>
     <row r="16">
@@ -1078,16 +1078,16 @@
         <v>5473972.9</v>
       </c>
       <c r="I16" t="n">
-        <v>340563.6371802762</v>
+        <v>267187.0574480658</v>
       </c>
       <c r="J16" t="n">
-        <v>548591.9163654803</v>
+        <v>610191.4122149925</v>
       </c>
       <c r="K16" t="n">
-        <v>357483.8294465155</v>
+        <v>283123.2977811521</v>
       </c>
       <c r="L16" t="n">
-        <v>563179.676998171</v>
+        <v>624750.5293215535</v>
       </c>
     </row>
     <row r="17">
@@ -1118,16 +1118,16 @@
         <v>66439271.8</v>
       </c>
       <c r="I17" t="n">
-        <v>4963163.004951928</v>
+        <v>4862420.20075058</v>
       </c>
       <c r="J17" t="n">
-        <v>5052236.066395054</v>
+        <v>5104014.293088192</v>
       </c>
       <c r="K17" t="n">
-        <v>5173720.225885791</v>
+        <v>5060732.987264478</v>
       </c>
       <c r="L17" t="n">
-        <v>5233768.184360191</v>
+        <v>5285189.967038705</v>
       </c>
     </row>
     <row r="18">
@@ -1158,16 +1158,16 @@
         <v>2058634.6</v>
       </c>
       <c r="I18" t="n">
-        <v>78314.12625614123</v>
+        <v>18244.77936770647</v>
       </c>
       <c r="J18" t="n">
-        <v>293619.0807423709</v>
+        <v>351556.5911197374</v>
       </c>
       <c r="K18" t="n">
-        <v>82063.17761801128</v>
+        <v>21775.81392001805</v>
       </c>
       <c r="L18" t="n">
-        <v>296851.3291120155</v>
+        <v>354782.4928681996</v>
       </c>
     </row>
     <row r="19">
@@ -1198,16 +1198,16 @@
         <v>2965009.3</v>
       </c>
       <c r="I19" t="n">
-        <v>180786.4775225116</v>
+        <v>141409.6994605679</v>
       </c>
       <c r="J19" t="n">
-        <v>304644.988253501</v>
+        <v>339741.1544963364</v>
       </c>
       <c r="K19" t="n">
-        <v>187989.0517091554</v>
+        <v>148193.4257592498</v>
       </c>
       <c r="L19" t="n">
-        <v>310854.6947698744</v>
+        <v>345938.6680589496</v>
       </c>
     </row>
     <row r="20">
@@ -1238,16 +1238,16 @@
         <v>696386.9</v>
       </c>
       <c r="I20" t="n">
-        <v>-17456.67666423059</v>
+        <v>-16494.53329866743</v>
       </c>
       <c r="J20" t="n">
-        <v>157925.8720691973</v>
+        <v>186838.0016695139</v>
       </c>
       <c r="K20" t="n">
-        <v>-32437.77458950738</v>
+        <v>-30604.44252629921</v>
       </c>
       <c r="L20" t="n">
-        <v>145009.90355595</v>
+        <v>173947.3940660673</v>
       </c>
     </row>
     <row r="21">
@@ -1278,16 +1278,16 @@
         <v>4430108.100000001</v>
       </c>
       <c r="I21" t="n">
-        <v>316413.0294681534</v>
+        <v>236423.1070006753</v>
       </c>
       <c r="J21" t="n">
-        <v>378478.151175689</v>
+        <v>418145.2731253565</v>
       </c>
       <c r="K21" t="n">
-        <v>351721.6155705319</v>
+        <v>269678.4096056995</v>
       </c>
       <c r="L21" t="n">
-        <v>408919.4838884365</v>
+        <v>448526.833325315</v>
       </c>
     </row>
     <row r="22">
@@ -1318,16 +1318,16 @@
         <v>18877626.9</v>
       </c>
       <c r="I22" t="n">
-        <v>1217182.496034731</v>
+        <v>1165508.357386678</v>
       </c>
       <c r="J22" t="n">
-        <v>1558854.309845584</v>
+        <v>1634801.384678124</v>
       </c>
       <c r="K22" t="n">
-        <v>1332105.318990719</v>
+        <v>1273748.127808059</v>
       </c>
       <c r="L22" t="n">
-        <v>1657935.136241398</v>
+        <v>1733687.662759685</v>
       </c>
     </row>
     <row r="23">
@@ -1358,16 +1358,16 @@
         <v>5996008.7</v>
       </c>
       <c r="I23" t="n">
-        <v>345007.2752979537</v>
+        <v>305560.2192948392</v>
       </c>
       <c r="J23" t="n">
-        <v>594840.5843203764</v>
+        <v>650982.9138272291</v>
       </c>
       <c r="K23" t="n">
-        <v>363157.8605393626</v>
+        <v>322655.30214271</v>
       </c>
       <c r="L23" t="n">
-        <v>610489.1294833784</v>
+        <v>666600.7325803621</v>
       </c>
     </row>
     <row r="24">
@@ -1398,16 +1398,16 @@
         <v>41599229.1</v>
       </c>
       <c r="I24" t="n">
-        <v>2938349.502330228</v>
+        <v>2852475.818426631</v>
       </c>
       <c r="J24" t="n">
-        <v>3051552.414554774</v>
+        <v>3101908.486522131</v>
       </c>
       <c r="K24" t="n">
-        <v>3236873.312004515</v>
+        <v>3133639.714277288</v>
       </c>
       <c r="L24" t="n">
-        <v>3308925.014709945</v>
+        <v>3358775.727494132</v>
       </c>
     </row>
     <row r="25">
@@ -1438,16 +1438,16 @@
         <v>11193380</v>
       </c>
       <c r="I25" t="n">
-        <v>804529.5289012053</v>
+        <v>747769.7197323454</v>
       </c>
       <c r="J25" t="n">
-        <v>938342.8827898689</v>
+        <v>981469.8207064534</v>
       </c>
       <c r="K25" t="n">
-        <v>830708.7714653428</v>
+        <v>772426.5731933251</v>
       </c>
       <c r="L25" t="n">
-        <v>960913.3428686697</v>
+        <v>1003995.962978066</v>
       </c>
     </row>
     <row r="26">
@@ -1478,16 +1478,16 @@
         <v>21062035.5</v>
       </c>
       <c r="I26" t="n">
-        <v>1502309.737173407</v>
+        <v>1426825.30690537</v>
       </c>
       <c r="J26" t="n">
-        <v>1583199.194522034</v>
+        <v>1624356.430168747</v>
       </c>
       <c r="K26" t="n">
-        <v>1640205.554673019</v>
+        <v>1556702.134190955</v>
       </c>
       <c r="L26" t="n">
-        <v>1702086.211068959</v>
+        <v>1743010.008325046</v>
       </c>
     </row>
     <row r="27">
@@ -1518,16 +1518,16 @@
         <v>9583869.9</v>
       </c>
       <c r="I27" t="n">
-        <v>663822.6393703439</v>
+        <v>596438.2140163889</v>
       </c>
       <c r="J27" t="n">
-        <v>772508.5937741785</v>
+        <v>815335.9143480232</v>
       </c>
       <c r="K27" t="n">
-        <v>725928.4431966752</v>
+        <v>654932.4084252042</v>
       </c>
       <c r="L27" t="n">
-        <v>826053.1744659165</v>
+        <v>868775.3585740097</v>
       </c>
     </row>
     <row r="28">
@@ -1558,16 +1558,16 @@
         <v>6007648.9</v>
       </c>
       <c r="I28" t="n">
-        <v>460304.4487496026</v>
+        <v>422831.5099067052</v>
       </c>
       <c r="J28" t="n">
-        <v>437161.9777700024</v>
+        <v>447031.634790507</v>
       </c>
       <c r="K28" t="n">
-        <v>497050.3756908738</v>
+        <v>457440.5683490587</v>
       </c>
       <c r="L28" t="n">
-        <v>468842.5153201084</v>
+        <v>478649.9666102086</v>
       </c>
     </row>
     <row r="29">
@@ -1598,16 +1598,16 @@
         <v>2287052.9</v>
       </c>
       <c r="I29" t="n">
-        <v>144938.1798733206</v>
+        <v>84231.64972324873</v>
       </c>
       <c r="J29" t="n">
-        <v>243091.1212682209</v>
+        <v>281713.8921881712</v>
       </c>
       <c r="K29" t="n">
-        <v>157583.0775120993</v>
+        <v>96141.21461400544</v>
       </c>
       <c r="L29" t="n">
-        <v>253992.9323751452</v>
+        <v>292594.2972466165</v>
       </c>
     </row>
     <row r="30">
@@ -1638,16 +1638,16 @@
         <v>51444246.7</v>
       </c>
       <c r="I30" t="n">
-        <v>3862354.681268951</v>
+        <v>3787042.244251377</v>
       </c>
       <c r="J30" t="n">
-        <v>3992976.257206521</v>
+        <v>4042368.871669999</v>
       </c>
       <c r="K30" t="n">
-        <v>3969987.03462275</v>
+        <v>3888415.504299033</v>
       </c>
       <c r="L30" t="n">
-        <v>4085771.597965813</v>
+        <v>4134982.005863479</v>
       </c>
     </row>
     <row r="31">
@@ -1678,16 +1678,16 @@
         <v>11157720.2</v>
       </c>
       <c r="I31" t="n">
-        <v>697756.4932251456</v>
+        <v>650385.7980818446</v>
       </c>
       <c r="J31" t="n">
-        <v>1005121.583601501</v>
+        <v>1073767.252441964</v>
       </c>
       <c r="K31" t="n">
-        <v>741479.5734825673</v>
+        <v>691566.270745585</v>
       </c>
       <c r="L31" t="n">
-        <v>1042817.480839728</v>
+        <v>1111389.132602127</v>
       </c>
     </row>
     <row r="32">
@@ -1718,16 +1718,16 @@
         <v>9568835.1</v>
       </c>
       <c r="I32" t="n">
-        <v>645064.5099081056</v>
+        <v>602816.4688153502</v>
       </c>
       <c r="J32" t="n">
-        <v>808401.6132561839</v>
+        <v>851137.3783889906</v>
       </c>
       <c r="K32" t="n">
-        <v>685420.9271483443</v>
+        <v>640826.0584230279</v>
       </c>
       <c r="L32" t="n">
-        <v>843194.9386174001</v>
+        <v>885862.3859631785</v>
       </c>
     </row>
     <row r="33">
@@ -1758,16 +1758,16 @@
         <v>74949539.5</v>
       </c>
       <c r="I33" t="n">
-        <v>6070540.840771213</v>
+        <v>5940850.042957444</v>
       </c>
       <c r="J33" t="n">
-        <v>6165426.968342058</v>
+        <v>6228782.625342092</v>
       </c>
       <c r="K33" t="n">
-        <v>5799290.713413681</v>
+        <v>5685373.795883409</v>
       </c>
       <c r="L33" t="n">
-        <v>5931568.400589623</v>
+        <v>5995383.246231748</v>
       </c>
     </row>
     <row r="34">
@@ -1798,16 +1798,16 @@
         <v>47903632.7</v>
       </c>
       <c r="I34" t="n">
-        <v>3278732.223371351</v>
+        <v>3177123.64608264</v>
       </c>
       <c r="J34" t="n">
-        <v>3538459.358699251</v>
+        <v>3619030.517815856</v>
       </c>
       <c r="K34" t="n">
-        <v>3670344.18377064</v>
+        <v>3545962.381484392</v>
       </c>
       <c r="L34" t="n">
-        <v>3876088.000815937</v>
+        <v>3955996.215490545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>